<commit_message>
tidied up data table from problem 6
</commit_message>
<xml_diff>
--- a/data/survey-data.xlsx
+++ b/data/survey-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsokolov/Documents/tfcb-homework01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9955A75-E749-F74F-9752-7F49C6BEDAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="1220" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="Tidy Table" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -140,16 +141,38 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t>Field Season</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Scale Calibrated?</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>note: 5 incorrect dates in 2014 plot 4 have been excluded and replaced by NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,6 +210,11 @@
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,6 +368,21 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +774,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,7 +818,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -800,7 +843,7 @@
   <dimension ref="C3:AB28"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -1410,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView topLeftCell="A2" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -2286,4 +2329,1425 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E0AD43-270C-6946-B117-FC86C168C4C6}">
+  <dimension ref="A1:G135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="22">
+        <v>41471</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22">
+        <v>41471</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>33</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="22">
+        <v>41471</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>2013</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22">
+        <v>41471</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2013</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="22">
+        <v>41473</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2013</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="22">
+        <v>41473</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>48</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="22">
+        <v>41473</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>29</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2013</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" s="22">
+        <v>41473</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>37</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2013</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22">
+        <v>41505</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>52</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2013</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="22">
+        <v>41564</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>33</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="22">
+        <v>41564</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15" s="22">
+        <v>41618</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="22">
+        <v>41618</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>45</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" s="22">
+        <v>41619</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>41</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2013</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18" s="22">
+        <v>41590</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>117</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2013</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>126</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>132</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>113</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>122</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>2013</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>107</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>2013</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" s="22">
+        <v>41591</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>115</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="22">
+        <v>41648</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="22">
+        <v>41648</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>36</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="22">
+        <v>41711</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>51</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>2014</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="22">
+        <v>41711</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>44</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="22">
+        <v>41711</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>146</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>44</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>7</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>45</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>157</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" s="22">
+        <v>41647</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" s="22">
+        <v>41688</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>218</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" s="22">
+        <v>41688</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>7</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="22">
+        <v>41688</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>52</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="22">
+        <v>41709</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>2014</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" s="22">
+        <v>41737</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>2014</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" s="22">
+        <v>41765</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>2014</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" s="22">
+        <v>41777</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>182</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" s="22">
+        <v>41799</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>29</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>2014</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" s="22">
+        <v>41828</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>115</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>2014</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="22">
+        <v>41828</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>190</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>2014</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>37</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>2014</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>2014</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>48</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>2014</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>52</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>2014</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>35</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C53" s="22"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C55" s="22"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C57" s="22"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C59" s="22"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C61" s="22"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C62" s="22"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C63" s="22"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C65" s="22"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C66" s="22"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C67" s="22"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C68" s="22"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C69" s="22"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C71" s="22"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C72" s="22"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C73" s="22"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C74" s="22"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C75" s="22"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C76" s="22"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C77" s="22"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C78" s="22"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C79" s="22"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C80" s="22"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C81" s="22"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C82" s="22"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C83" s="22"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C84" s="22"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C85" s="22"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C86" s="22"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C87" s="22"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C88" s="22"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C89" s="22"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C90" s="22"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C91" s="22"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C93" s="22"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C95" s="22"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C97" s="22"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C101" s="22"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C102" s="22"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C103" s="22"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C104" s="22"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C105" s="22"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C106" s="22"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C107" s="22"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C108" s="22"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C109" s="22"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C111" s="22"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C112" s="22"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C113" s="22"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C114" s="22"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C115" s="22"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C116" s="22"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C117" s="22"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C118" s="22"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C119" s="22"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C120" s="22"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C121" s="22"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C122" s="22"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C123" s="22"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C124" s="22"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C125" s="22"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C126" s="22"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C127" s="22"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C128" s="22"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C129" s="22"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C130" s="22"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C131" s="22"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C132" s="22"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C133" s="22"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C134" s="22"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C135" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>